<commit_message>
Added temp and pressure values
</commit_message>
<xml_diff>
--- a/Lab_2/Lab2_Data.xlsx
+++ b/Lab_2/Lab2_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test No</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>PT2</t>
+  </si>
+  <si>
+    <t>Temp (F)</t>
+  </si>
+  <si>
+    <t>Pressure  (kPa)</t>
   </si>
 </sst>
 </file>
@@ -384,14 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,7 +476,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A11" si="1">A3+1</f>
+        <f t="shared" ref="A4:A10" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -640,6 +647,22 @@
       </c>
       <c r="G10" s="1">
         <v>1.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>100.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All data calculations complete, finished first two graphs
</commit_message>
<xml_diff>
--- a/Lab_2/Lab2_Data.xlsx
+++ b/Lab_2/Lab2_Data.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="9270"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="9270" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Efficiency vs Re" sheetId="4" r:id="rId1"/>
+    <sheet name="Power Coefficient vs Re" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="Area2">Sheet1!$L$7</definedName>
+    <definedName name="beta">Sheet1!$L$8</definedName>
+    <definedName name="Cd">Sheet1!$L$12</definedName>
+    <definedName name="Cd2_">Sheet1!$L$13</definedName>
+    <definedName name="Cd3_">Sheet1!$L$14</definedName>
+    <definedName name="density">Sheet1!$L$4</definedName>
+    <definedName name="density_w">Sheet1!$L$5</definedName>
+    <definedName name="mu">Sheet1!$L$6</definedName>
+    <definedName name="P_static">Sheet1!$L$3</definedName>
+    <definedName name="Re">Sheet1!$L$9</definedName>
+    <definedName name="Re2_">Sheet1!$L$10</definedName>
+    <definedName name="Re3_">Sheet1!$L$11</definedName>
+    <definedName name="temp">Sheet1!$L$2</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Test No</t>
   </si>
@@ -33,29 +50,110 @@
     <t xml:space="preserve">HP </t>
   </si>
   <si>
-    <t>PT1</t>
-  </si>
-  <si>
-    <t>PT2</t>
-  </si>
-  <si>
-    <t>Temp (F)</t>
-  </si>
-  <si>
-    <t>Pressure  (kPa)</t>
+    <t>PT1 (in)</t>
+  </si>
+  <si>
+    <t>PT2 (in)</t>
+  </si>
+  <si>
+    <t>Power Input (ft lb / sec)</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>Static Pressure (Pa)</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>Temp (K)</t>
+  </si>
+  <si>
+    <t>Air Density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>μ (kg/m s)</t>
+  </si>
+  <si>
+    <t>Power Output (W)</t>
+  </si>
+  <si>
+    <t>Power Input (W)</t>
+  </si>
+  <si>
+    <t>Q (m^3/s)</t>
+  </si>
+  <si>
+    <t>Water Density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>PT1 (m)</t>
+  </si>
+  <si>
+    <t>PT2 (m)</t>
+  </si>
+  <si>
+    <t>A2 (m^2)</t>
+  </si>
+  <si>
+    <t>ΔP1 (Pa)</t>
+  </si>
+  <si>
+    <t>ΔP2 (Pa)</t>
+  </si>
+  <si>
+    <t>Cp</t>
+  </si>
+  <si>
+    <t>Cw</t>
+  </si>
+  <si>
+    <t>Cq</t>
+  </si>
+  <si>
+    <t>Re2</t>
+  </si>
+  <si>
+    <t>Re3</t>
+  </si>
+  <si>
+    <t>Cd2</t>
+  </si>
+  <si>
+    <t>Cd3</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,16 +191,753 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" u="sng">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Compression</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" u="sng" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Efficiency vs. Reynold's Number for Each Plate Distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" u="sng">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3551145133518158E-2"/>
+          <c:y val="1.4117647806135E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>X = 3 Inches</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>423520.46671442688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>697222.79136540578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$27:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>X = 2 Inches</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$30:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>445631.8610974992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>701735.60735360405</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$30:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.15146627692261169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24866340664051401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30690642829838921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>X = 1 Inch</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$33:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>466696.82399223116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>674205.76358894468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$33:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.514662769226117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48929490990351959</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53803235044911879</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="167271040"/>
+        <c:axId val="175870336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="167271040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Re</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="175870336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="175870336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>η</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4634146903558552E-2"/>
+              <c:y val="0.41872848110783994"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="167271040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" u="sng">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Power Coefficient </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" u="sng" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>vs. Reynold's Number for Each Plate Distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" u="sng">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10599017115383795"/>
+          <c:y val="1.6134454635582857E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>X = 3 Inches</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>423520.46671442688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>697222.79136540578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.7543283335532624E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6091592067524444E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.508425306132502E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>X = 2 Inches</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$30:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>445631.8610974992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>701735.60735360405</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$30:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.8267574364567045E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1772531751768856E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2888671592087111E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>X = 1 Inch</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$33:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>216040.80447566588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>466696.82399223116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>674205.76358894468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$33:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.6535148729134082E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3500785595087558E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2763790873205791E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146785792"/>
+        <c:axId val="146787712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146785792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Re</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146787712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146787712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Cw</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4634146903558552E-2"/>
+              <c:y val="0.41872848110783994"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146785792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8678333" cy="6297083"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8678333" cy="6297083"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -180,6 +1015,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -214,6 +1050,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,20 +1226,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B27" sqref="B27:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,13 +1262,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -442,14 +1285,23 @@
         <f>D2*(B2/4000)</f>
         <v>7.8875000000000001E-2</v>
       </c>
-      <c r="F2" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="2">
+        <f>K17*0.0254</f>
+        <v>8.8899999999999986E-3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>L17*0.0254</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="9">
+        <f>(70-32)*(5/9)+273</f>
+        <v>294.11111111111109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -467,14 +1319,22 @@
         <f t="shared" ref="E3:E10" si="0">D3*(B3/4000)</f>
         <v>0.52674999999999994</v>
       </c>
-      <c r="F3" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3" s="2">
+        <f>K18*0.0254</f>
+        <v>3.5559999999999994E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <f>L18*0.0254</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>100250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A10" si="1">A3+1</f>
         <v>3</v>
@@ -492,14 +1352,23 @@
         <f t="shared" si="0"/>
         <v>1.7774249999999998</v>
       </c>
-      <c r="F4" s="1">
-        <v>3.85</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="2">
+        <f>K19*0.0254</f>
+        <v>9.7790000000000002E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f>L19*0.0254</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="10">
+        <f>P_static/(287*temp)</f>
+        <v>1.1876570543998928</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -517,14 +1386,22 @@
         <f t="shared" si="0"/>
         <v>7.8125E-2</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="2">
+        <f>K20*0.0254</f>
+        <v>8.8899999999999986E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <f>L20*0.0254</f>
+        <v>2.5400000000000002E-3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -542,14 +1419,23 @@
         <f t="shared" si="0"/>
         <v>0.49080000000000007</v>
       </c>
-      <c r="F6" s="1">
-        <v>1.55</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="2">
+        <f>K21*0.0254</f>
+        <v>3.9370000000000002E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <f>L21*0.0254</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <f>1.983*10^-5</f>
+        <v>1.9830000000000002E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -567,14 +1453,23 @@
         <f t="shared" si="0"/>
         <v>1.6280999999999999</v>
       </c>
-      <c r="F7" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" s="2">
+        <f>K22*0.0254</f>
+        <v>9.9059999999999995E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f>L22*0.0254</f>
+        <v>3.3020000000000001E-2</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="8">
+        <f>(PI()*18^2)/(4*144)*0.0254</f>
+        <v>4.4885505038164165E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -592,14 +1487,22 @@
         <f t="shared" si="0"/>
         <v>1.5625E-2</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="2">
+        <f>K23*0.0254</f>
+        <v>8.8899999999999986E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <f>L23*0.0254</f>
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -617,14 +1520,22 @@
         <f t="shared" si="0"/>
         <v>0.41795000000000004</v>
       </c>
-      <c r="F9" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="2">
+        <f>K24*0.0254</f>
+        <v>4.3179999999999996E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f>L24*0.0254</f>
+        <v>2.0320000000000001E-2</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="14">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -642,27 +1553,691 @@
         <f t="shared" si="0"/>
         <v>1.1325000000000001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
+        <f>K25*0.0254</f>
+        <v>9.1439999999999994E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f>L25*0.0254</f>
+        <v>4.1909999999999996E-2</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10">
+        <v>430000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11">
+        <v>690000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="8">
+        <f>0.5959+0.0312*beta^2.1-0.184*beta^8+0.029*beta^2.5*(10^6/Re)+(0.09*1*beta^4/(1-beta^5))-0.037*0.5*beta^3</f>
+        <v>0.63036487877356873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="8">
+        <f>0.5959+0.0312*beta^2.1-0.184*beta^8+0.029*beta^2.5*(10^6/Re2_)+(0.09*1*beta^4/(1-beta^5))-0.037*0.5*beta^3</f>
+        <v>0.61787500816457053</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="8">
+        <f>0.5959+0.0312*beta^2.1-0.184*beta^8+0.029*beta^2.5*(10^6/Re3_)+(0.09*1*beta^4/(1-beta^5))-0.037*0.5*beta^3</f>
+        <v>0.61338260411153156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7.8875000000000001E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B16*550</f>
+        <v>43.381250000000001</v>
+      </c>
+      <c r="D16" s="4">
+        <f>C16*1.355818</f>
+        <v>58.817079612500002</v>
+      </c>
+      <c r="E16" s="5">
+        <f>9.81*F2*density_w</f>
+        <v>87.210899999999995</v>
+      </c>
+      <c r="F16" s="5">
+        <f>9.81*G2*density_w</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <f>Cd*Area2*SQRT((2*E16)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.35413376908105576</v>
+      </c>
+      <c r="H16" s="1">
+        <f>G16*F16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f>A16+1</f>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.52674999999999994</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" ref="C17:C24" si="2">B17*550</f>
+        <v>289.71249999999998</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" ref="D17:D24" si="3">C17*1.355818</f>
+        <v>392.79742232499996</v>
+      </c>
+      <c r="E17" s="5">
+        <f>9.81*F3*density_w</f>
+        <v>348.84359999999998</v>
+      </c>
+      <c r="F17" s="5">
+        <f>9.81*G3*density_w</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <f>Cd2_*Area2*SQRT((2*E17)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.69423412639366167</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17:H24" si="4">G17*F17</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" ref="A18:A24" si="5">A17+1</f>
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.7774249999999998</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="2"/>
+        <v>977.5837499999999</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="3"/>
+        <v>1325.4256447574999</v>
+      </c>
+      <c r="E18" s="5">
+        <f>9.81*F4*density_w</f>
+        <v>959.31990000000008</v>
+      </c>
+      <c r="F18" s="5">
+        <f>9.81*G4*density_w</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <f>Cd3_*Area2*SQRT((2*E18)/density)*SQRT(1/(1-beta^4))</f>
+        <v>1.1428865745741883</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="2"/>
+        <v>42.96875</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="3"/>
+        <v>58.257804687499998</v>
+      </c>
+      <c r="E19" s="5">
+        <f>9.81*F5*density_w</f>
+        <v>87.210899999999995</v>
+      </c>
+      <c r="F19" s="5">
+        <f>9.81*G5*density_w</f>
+        <v>24.917400000000004</v>
+      </c>
+      <c r="G19" s="4">
+        <f>Cd*Area2*SQRT((2*E19)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.35413376908105576</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="4"/>
+        <v>8.8240927777003009</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.49080000000000007</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="2"/>
+        <v>269.94000000000005</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="3"/>
+        <v>365.98951092000004</v>
+      </c>
+      <c r="E20" s="5">
+        <f>9.81*F6*density_w</f>
+        <v>386.21970000000005</v>
+      </c>
+      <c r="F20" s="5">
+        <f>9.81*G6*density_w</f>
+        <v>124.587</v>
+      </c>
+      <c r="G20" s="4">
+        <f>Cd2_*Area2*SQRT((2*E20)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.73047909155901347</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="4"/>
+        <v>91.00819858006281</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.6280999999999999</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="2"/>
+        <v>895.45499999999993</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="3"/>
+        <v>1214.07400719</v>
+      </c>
+      <c r="E21" s="5">
+        <f>9.81*F7*density_w</f>
+        <v>971.7786000000001</v>
+      </c>
+      <c r="F21" s="5">
+        <f>9.81*G7*density_w</f>
+        <v>323.92619999999999</v>
+      </c>
+      <c r="G21" s="4">
+        <f>Cd3_*Area2*SQRT((2*E21)/density)*SQRT(1/(1-beta^4))</f>
+        <v>1.1502839759074623</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="4"/>
+        <v>372.6071172365958</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1.55</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="2"/>
+        <v>8.59375</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="3"/>
+        <v>11.651560937499999</v>
+      </c>
+      <c r="E22" s="5">
+        <f>9.81*F8*density_w</f>
+        <v>87.210899999999995</v>
+      </c>
+      <c r="F22" s="5">
+        <f>9.81*G8*density_w</f>
+        <v>49.834800000000008</v>
+      </c>
+      <c r="G22" s="4">
+        <f>Cd*Area2*SQRT((2*E22)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.35413376908105576</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="4"/>
+        <v>17.648185555400602</v>
+      </c>
+      <c r="K22" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.41795000000000004</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="2"/>
+        <v>229.87250000000003</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="3"/>
+        <v>311.66527320500006</v>
+      </c>
+      <c r="E23" s="5">
+        <f>9.81*F9*density_w</f>
+        <v>423.59579999999994</v>
+      </c>
+      <c r="F23" s="5">
+        <f>9.81*G9*density_w</f>
+        <v>199.33920000000003</v>
+      </c>
+      <c r="G23" s="4">
+        <f>Cd2_*Area2*SQRT((2*E23)/density)*SQRT(1/(1-beta^4))</f>
+        <v>0.76500874776710404</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="4"/>
+        <v>152.49623177289632</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.1325000000000001</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="2"/>
+        <v>622.875</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="3"/>
+        <v>844.50513675000002</v>
+      </c>
+      <c r="E24" s="5">
+        <f>9.81*F10*density_w</f>
+        <v>897.02639999999997</v>
+      </c>
+      <c r="F24" s="5">
+        <f>9.81*G10*density_w</f>
+        <v>411.13709999999998</v>
+      </c>
+      <c r="G24" s="4">
+        <f>Cd3_*Area2*SQRT((2*E24)/density)*SQRT(1/(1-beta^4))</f>
+        <v>1.1051570964818234</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="4"/>
+        <v>454.37108369195704</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" s="1">
         <v>3.6</v>
       </c>
-      <c r="G10" s="1">
+      <c r="L25" s="1">
         <v>1.65</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="11">
+        <f>D16/(density*((2*PI()*B2)/60)^3*(18*0.0254))</f>
+        <v>3.7543283335532624E-4</v>
+      </c>
+      <c r="C27" s="2">
+        <f>E16/(density*((2*PI()*B2)/60)^2*(18*0.0254)^2)</f>
+        <v>8.0454681102905851E-2</v>
+      </c>
+      <c r="D27" s="3">
+        <f>G16/(((2*PI()*B2)/60)*(18*0.0254)^3)</f>
+        <v>5.6077765382437458E-2</v>
+      </c>
+      <c r="E27" s="13">
+        <f>(density*(G16/Area2)*(18*0.0254))/mu</f>
+        <v>216040.80447566588</v>
+      </c>
+      <c r="F27" s="1">
+        <f>H16/D16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f>A27+1</f>
+        <v>2</v>
+      </c>
+      <c r="B28" s="11">
+        <f>D17/(density*((2*PI()*B3)/60)^3*(18*0.0254))</f>
+        <v>3.6091592067524444E-4</v>
+      </c>
+      <c r="C28" s="2">
+        <f>E17/(density*((2*PI()*B3)/60)^2*(18*0.0254)^2)</f>
+        <v>8.8392833088525802E-2</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" ref="D28:D35" si="6">G17/(((2*PI()*B3)/60)*(18*0.0254)^3)</f>
+        <v>5.7614551883381562E-2</v>
+      </c>
+      <c r="E28" s="13">
+        <f>(density*(G17/Area2)*(18*0.0254))/mu</f>
+        <v>423520.46671442688</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" ref="F28:F35" si="7">H17/D17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" ref="A29:A35" si="8">A28+1</f>
+        <v>3</v>
+      </c>
+      <c r="B29" s="11">
+        <f>D18/(density*((2*PI()*B4)/60)^3*(18*0.0254))</f>
+        <v>3.508425306132502E-4</v>
+      </c>
+      <c r="C29" s="2">
+        <f>E18/(density*((2*PI()*B4)/60)^2*(18*0.0254)^2)</f>
+        <v>0.1060301520279079</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="6"/>
+        <v>6.2642514085770221E-2</v>
+      </c>
+      <c r="E29" s="13">
+        <f>(density*(G18/Area2)*(18*0.0254))/mu</f>
+        <v>697222.79136540578</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="11">
+        <f>D19/(density*((2*PI()*B5)/60)^3*(18*0.0254))</f>
+        <v>3.8267574364567045E-4</v>
+      </c>
+      <c r="C30" s="2">
+        <f>E19/(density*((2*PI()*B5)/60)^2*(18*0.0254)^2)</f>
+        <v>8.2006825683492088E-2</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="6"/>
+        <v>5.6616111930108862E-2</v>
+      </c>
+      <c r="E30" s="13">
+        <f>(density*(G19/Area2)*(18*0.0254))/mu</f>
+        <v>216040.80447566588</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="7"/>
+        <v>0.15146627692261169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="11">
+        <f>D20/(density*((2*PI()*B6)/60)^3*(18*0.0254))</f>
+        <v>3.1772531751768856E-4</v>
+      </c>
+      <c r="C31" s="2">
+        <f>E20/(density*((2*PI()*B6)/60)^2*(18*0.0254)^2)</f>
+        <v>9.4228996183025299E-2</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="6"/>
+        <v>5.948616122058447E-2</v>
+      </c>
+      <c r="E31" s="13">
+        <f>(density*(G20/Area2)*(18*0.0254))/mu</f>
+        <v>445631.8610974992</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="7"/>
+        <v>0.24866340664051401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="11">
+        <f>D21/(density*((2*PI()*B7)/60)^3*(18*0.0254))</f>
+        <v>3.2888671592087111E-4</v>
+      </c>
+      <c r="C32" s="2">
+        <f>E21/(density*((2*PI()*B7)/60)^2*(18*0.0254)^2)</f>
+        <v>0.10907606579332753</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="6"/>
+        <v>6.3535904928513826E-2</v>
+      </c>
+      <c r="E32" s="13">
+        <f>(density*(G21/Area2)*(18*0.0254))/mu</f>
+        <v>701735.60735360405</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="7"/>
+        <v>0.30690642829838921</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="B12">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+      <c r="B33" s="11">
+        <f>D22/(density*((2*PI()*B8)/60)^3*(18*0.0254))</f>
+        <v>7.6535148729134082E-5</v>
+      </c>
+      <c r="C33" s="2">
+        <f>E22/(density*((2*PI()*B8)/60)^2*(18*0.0254)^2)</f>
+        <v>8.2006825683492088E-2</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="6"/>
+        <v>5.6616111930108862E-2</v>
+      </c>
+      <c r="E33" s="13">
+        <f>(density*(G22/Area2)*(18*0.0254))/mu</f>
+        <v>216040.80447566588</v>
+      </c>
+      <c r="F33" s="3">
+        <f>H22/D22</f>
+        <v>1.514662769226117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="B13">
-        <v>100.25</v>
+      <c r="B34" s="11">
+        <f>D23/(density*((2*PI()*B9)/60)^3*(18*0.0254))</f>
+        <v>2.3500785595087558E-4</v>
+      </c>
+      <c r="C34" s="2">
+        <f>E23/(density*((2*PI()*B9)/60)^2*(18*0.0254)^2)</f>
+        <v>9.4082527505454927E-2</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="6"/>
+        <v>5.9439910872221877E-2</v>
+      </c>
+      <c r="E34" s="13">
+        <f>(density*(G23/Area2)*(18*0.0254))/mu</f>
+        <v>466696.82399223116</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="7"/>
+        <v>0.48929490990351959</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="B35" s="11">
+        <f>D24/(density*((2*PI()*B10)/60)^3*(18*0.0254))</f>
+        <v>2.2763790873205791E-4</v>
+      </c>
+      <c r="C35" s="2">
+        <f>E24/(density*((2*PI()*B10)/60)^2*(18*0.0254)^2)</f>
+        <v>0.10035247916010605</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="6"/>
+        <v>6.0942257835026686E-2</v>
+      </c>
+      <c r="E35" s="13">
+        <f>(density*(G24/Area2)*(18*0.0254))/mu</f>
+        <v>674205.76358894468</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="7"/>
+        <v>0.53803235044911879</v>
       </c>
     </row>
   </sheetData>
@@ -671,24 +2246,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>